<commit_message>
update output data and maps
</commit_message>
<xml_diff>
--- a/pearson_tables/t2m_netherlands-2-10.xlsx
+++ b/pearson_tables/t2m_netherlands-2-10.xlsx
@@ -457,13 +457,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.6605572307021658</v>
+        <v>-0.6594644287856457</v>
       </c>
       <c r="C2" t="n">
-        <v>0.530124507673613</v>
+        <v>0.5528200562108995</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4969126642239438</v>
+        <v>-0.5161509248614538</v>
       </c>
     </row>
     <row r="3">
@@ -473,13 +473,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6860316896959928</v>
+        <v>-0.7420218047750701</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6772407780093614</v>
+        <v>-0.7235027927716031</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.5843060624302807</v>
+        <v>-0.7217693428549651</v>
       </c>
     </row>
     <row r="4">
@@ -489,13 +489,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.6314882487995875</v>
+        <v>-0.6312246050722827</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5435527655585132</v>
+        <v>0.5532091562655042</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.4818601857390206</v>
+        <v>-0.09814806294152349</v>
       </c>
     </row>
     <row r="5">
@@ -505,13 +505,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.680837170400485</v>
+        <v>0.6670915658037653</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.6762380581763355</v>
+        <v>-0.6488536836452636</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5808075561735059</v>
+        <v>-0.5740329548498322</v>
       </c>
     </row>
     <row r="6">
@@ -521,13 +521,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.7568262096348543</v>
+        <v>0.8000244920464049</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7187607900921431</v>
+        <v>-0.6993995071951961</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.6325112134351196</v>
+        <v>-0.6619501785003117</v>
       </c>
     </row>
     <row r="7">
@@ -537,13 +537,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.6441549588559923</v>
+        <v>-0.6538899606634785</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6503929390860502</v>
+        <v>-0.6582497949293676</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.6974818185329164</v>
+        <v>0.6765693485992146</v>
       </c>
     </row>
     <row r="8">
@@ -553,13 +553,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.8128358182178775</v>
+        <v>-0.8353421471694314</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8981868089159656</v>
+        <v>0.8846250243691259</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.6681319729704147</v>
+        <v>0.6750595056807498</v>
       </c>
     </row>
     <row r="9">
@@ -569,13 +569,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.805675296627736</v>
+        <v>0.8023964163849941</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6982373391509229</v>
+        <v>0.7104722060248243</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6650394052066601</v>
+        <v>0.6738028332491574</v>
       </c>
     </row>
   </sheetData>

</xml_diff>